<commit_message>
Add function to transform & group field :sparkles:
</commit_message>
<xml_diff>
--- a/data-dictionary.xlsx
+++ b/data-dictionary.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Đại Học CNTT\Data engineer\DE-COURSE\Homework\Recruitment user behavior pipeline\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B01465E-2ADE-4697-8A13-EDBBA62CDAD8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{143F8FD6-9EC1-46B3-A0CA-7C7BE1646901}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5595" yWindow="2460" windowWidth="21600" windowHeight="13110" xr2:uid="{FC2D4DA4-C2AE-4DAA-BEF6-4B339A3C3E35}"/>
+    <workbookView xWindow="5940" yWindow="2805" windowWidth="21600" windowHeight="13110" xr2:uid="{FC2D4DA4-C2AE-4DAA-BEF6-4B339A3C3E35}"/>
   </bookViews>
   <sheets>
     <sheet name="Cassandra" sheetId="1" r:id="rId1"/>
@@ -556,8 +556,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C0165B9B-1760-4D03-90C1-42E88D75B8A6}">
   <dimension ref="A1:M30"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="G32" sqref="G32"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -582,7 +582,7 @@
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A2" s="3" t="s">
+      <c r="A2" s="4" t="s">
         <v>2</v>
       </c>
       <c r="B2" s="3" t="s">
@@ -742,7 +742,7 @@
       </c>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A13" s="3" t="s">
+      <c r="A13" s="4" t="s">
         <v>15</v>
       </c>
       <c r="B13" s="3" t="s">
@@ -810,7 +810,7 @@
       </c>
     </row>
     <row r="17" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A17" s="3" t="s">
+      <c r="A17" s="4" t="s">
         <v>19</v>
       </c>
       <c r="B17" s="3" t="s">
@@ -861,7 +861,7 @@
       </c>
     </row>
     <row r="20" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A20" s="3" t="s">
+      <c r="A20" s="4" t="s">
         <v>22</v>
       </c>
       <c r="B20" s="3" t="s">

</xml_diff>